<commit_message>
Use same kind of headers
Headers were of different types before. Now headers have the same length
and plating type.
</commit_message>
<xml_diff>
--- a/docs/a4000-bom.xlsx
+++ b/docs/a4000-bom.xlsx
@@ -1363,7 +1363,7 @@
     <t>12 Pin DIL Header</t>
   </si>
   <si>
-    <t>649-1012938191203BLF</t>
+    <t>649-67997-212HLF</t>
   </si>
   <si>
     <t>J975</t>
@@ -1387,7 +1387,7 @@
     <t>40 Pin DIL Header</t>
   </si>
   <si>
-    <t>649-861400402YO2LF</t>
+    <t>649-67997-240HLF</t>
   </si>
   <si>
     <t>CN900</t>
@@ -1399,7 +1399,7 @@
     <t>2 Pin SIL Header</t>
   </si>
   <si>
-    <t>649-1012937890203BLF</t>
+    <t>649-68001-202HLF</t>
   </si>
   <si>
     <t>J351 J850</t>
@@ -1411,7 +1411,7 @@
     <t>3 Pin SIL Header</t>
   </si>
   <si>
-    <t>649-1012937890303BLF</t>
+    <t>649-68001-203HLF</t>
   </si>
   <si>
     <t>CN200 CN302 CN303 CN404 J100 J104 J151 J212 J213 J214 J352 J500 J501 J502 J852</t>
@@ -1721,7 +1721,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Version: 0.10 (2021-05-08)
+      <t xml:space="preserve">Version: 0.11 (2021-05-10)
 </t>
     </r>
     <r>

</xml_diff>

<commit_message>
More filter bead details
Added impedance and current. Found a better part for 391092-03.
</commit_message>
<xml_diff>
--- a/docs/a4000-bom.xlsx
+++ b/docs/a4000-bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="564">
   <si>
     <t>Part Id</t>
   </si>
@@ -1270,7 +1270,7 @@
     <t>391559-01</t>
   </si>
   <si>
-    <t>Filter, Ferrite</t>
+    <t>47Ω @ 100MHz, 5A</t>
   </si>
   <si>
     <t>1812</t>
@@ -1285,7 +1285,10 @@
     <t>391092-03</t>
   </si>
   <si>
-    <t>623-2512061517Y3</t>
+    <t>600Ω @ 100MHz, 200mA</t>
+  </si>
+  <si>
+    <t>81-BLM31AJ601SH1L</t>
   </si>
   <si>
     <t>ER976 ER977 ER978 ER979 ER980 ER981 ER982 ER983 ER984 ER985 ER986 ER987 ER988 ER989 FB410 FB411 FB710</t>
@@ -1721,7 +1724,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Version: 0.11 (2021-05-10)
+      <t xml:space="preserve">Version: 0.12 (2021-05-10)
 </t>
     </r>
     <r>
@@ -4211,21 +4214,21 @@
         <v>17</v>
       </c>
       <c r="C107" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="E107" t="s">
         <v>225</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="2" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -4236,87 +4239,87 @@
     </row>
     <row r="109" spans="1:7">
       <c r="A109" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B109">
         <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E109" t="s">
         <v>58</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B110">
         <v>1</v>
       </c>
       <c r="C110" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D110" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E110" t="s">
         <v>58</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B111">
         <v>1</v>
       </c>
       <c r="C111" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D111" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="E111" t="s">
         <v>58</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B112">
         <v>1</v>
       </c>
       <c r="C112" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E112" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -4327,288 +4330,288 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B114">
         <v>5</v>
       </c>
       <c r="C114" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="115" spans="1:7">
       <c r="A115" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B115">
         <v>1</v>
       </c>
       <c r="C115" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="116" spans="1:7">
       <c r="A116" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B116">
         <v>1</v>
       </c>
       <c r="C116" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="117" spans="1:7">
       <c r="A117" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B117">
         <v>1</v>
       </c>
       <c r="C117" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="118" spans="1:7">
       <c r="A118" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B118">
         <v>2</v>
       </c>
       <c r="C118" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B119">
         <v>15</v>
       </c>
       <c r="C119" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="120" spans="1:7">
       <c r="A120" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B120">
         <v>2</v>
       </c>
       <c r="C120" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D120" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="121" spans="1:7">
       <c r="A121" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B121">
         <v>1</v>
       </c>
       <c r="C121" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D121" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="122" spans="1:7">
       <c r="A122" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B122">
         <v>1</v>
       </c>
       <c r="C122" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D122" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="123" spans="1:7">
       <c r="A123" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B123">
         <v>1</v>
       </c>
       <c r="C123" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="D123" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="124" spans="1:7">
       <c r="A124" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B124">
         <v>1</v>
       </c>
       <c r="C124" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="125" spans="1:7">
       <c r="A125" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B125">
         <v>1</v>
       </c>
       <c r="C125" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D125" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="126" spans="1:7">
       <c r="A126" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B126">
         <v>1</v>
       </c>
       <c r="C126" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D126" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="127" spans="1:7">
       <c r="A127" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B127">
         <v>1</v>
       </c>
       <c r="C127" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D127" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="F127" s="4" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="128" spans="1:7">
       <c r="A128" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B128">
         <v>2</v>
       </c>
       <c r="C128" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="129" spans="1:7">
       <c r="A129" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B129">
         <v>1</v>
       </c>
       <c r="C129" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="130" spans="1:7">
       <c r="A130" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -4619,22 +4622,22 @@
     </row>
     <row r="131" spans="1:7">
       <c r="A131" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B131">
         <v>8</v>
       </c>
       <c r="C131" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="D131" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="F131" s="4" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -4642,16 +4645,16 @@
         <v>1</v>
       </c>
       <c r="C132" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="D132" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="E132" t="s">
         <v>51</v>
       </c>
       <c r="F132" s="4" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="G132" s="3" t="s">
         <v>52</v>
@@ -4659,22 +4662,22 @@
     </row>
     <row r="133" spans="1:7">
       <c r="A133" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B133">
         <v>1</v>
       </c>
       <c r="C133" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D133" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="E133" t="s">
         <v>167</v>
       </c>
       <c r="F133" s="4" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="G133" s="3" t="s">
         <v>169</v>
@@ -4682,25 +4685,25 @@
     </row>
     <row r="134" spans="1:7">
       <c r="A134" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B134">
         <v>2</v>
       </c>
       <c r="C134" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="D134" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="E134" t="s">
         <v>44</v>
       </c>
       <c r="F134" s="4" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -4708,19 +4711,19 @@
         <v>5</v>
       </c>
       <c r="C135" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D135" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="E135" t="s">
         <v>69</v>
       </c>
       <c r="F135" s="4" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -4728,16 +4731,16 @@
         <v>1</v>
       </c>
       <c r="C136" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D136" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="E136" t="s">
         <v>63</v>
       </c>
       <c r="F136" s="4" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="G136" s="3" t="s">
         <v>65</v>
@@ -4748,19 +4751,19 @@
         <v>3</v>
       </c>
       <c r="C137" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D137" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E137" t="s">
         <v>25</v>
       </c>
       <c r="F137" s="4" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -4768,16 +4771,16 @@
         <v>1</v>
       </c>
       <c r="C138" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D138" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="E138" t="s">
         <v>21</v>
       </c>
       <c r="F138" s="4" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="G138" s="3" t="s">
         <v>22</v>
@@ -4788,24 +4791,24 @@
         <v>5</v>
       </c>
       <c r="C139" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="D139" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E139" t="s">
         <v>14</v>
       </c>
       <c r="F139" s="4" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="140" spans="1:7">
       <c r="A140" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -4816,84 +4819,84 @@
     </row>
     <row r="141" spans="1:7">
       <c r="A141" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B141">
         <v>1</v>
       </c>
       <c r="C141" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D141" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E141" t="s">
         <v>266</v>
       </c>
       <c r="F141" s="4" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="142" spans="1:7">
       <c r="A142" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B142">
         <v>1</v>
       </c>
       <c r="C142" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="F142" s="4" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="143" spans="1:7">
       <c r="A143" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B143">
         <v>1</v>
       </c>
       <c r="C143" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D143" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="144" spans="1:7">
       <c r="A144" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B144">
         <v>13</v>
       </c>
       <c r="C144" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D144" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="F144" s="4" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="60" customHeight="1">
       <c r="A146" s="5" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix package size on L500 example part
</commit_message>
<xml_diff>
--- a/docs/a4000-bom.xlsx
+++ b/docs/a4000-bom.xlsx
@@ -1660,7 +1660,7 @@
     <t>L500 can be left out on Acill boards</t>
   </si>
   <si>
-    <t>652-CC453232-470KL</t>
+    <t>963-CBC3225T470MRV</t>
   </si>
   <si>
     <t>L500</t>
@@ -1724,7 +1724,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Version: 0.12 (2021-05-10)
+      <t xml:space="preserve">Version: 0.13 (2021-05-12)
 </t>
     </r>
     <r>

</xml_diff>

<commit_message>
Add power plug parts to the list
</commit_message>
<xml_diff>
--- a/docs/a4000-bom.xlsx
+++ b/docs/a4000-bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="571">
   <si>
     <t>Part Id</t>
   </si>
@@ -1546,7 +1546,64 @@
     <t>CN651</t>
   </si>
   <si>
-    <t>Sockets</t>
+    <t>Various</t>
+  </si>
+  <si>
+    <t>391138-05</t>
+  </si>
+  <si>
+    <t>Inductor, 47µH</t>
+  </si>
+  <si>
+    <t>L500 can be left out on Acill boards</t>
+  </si>
+  <si>
+    <t>963-CBC3225T470MRV</t>
+  </si>
+  <si>
+    <t>L500</t>
+  </si>
+  <si>
+    <t>390924-01</t>
+  </si>
+  <si>
+    <t>Varistor Switch, Self Resetting 1.85A</t>
+  </si>
+  <si>
+    <t>652-MFR185</t>
+  </si>
+  <si>
+    <t>F175</t>
+  </si>
+  <si>
+    <t>380393-02</t>
+  </si>
+  <si>
+    <t>Battery, NiCd 3.6V 680mAh 3/60DK</t>
+  </si>
+  <si>
+    <t>Not recommended</t>
+  </si>
+  <si>
+    <t>BT176</t>
+  </si>
+  <si>
+    <t>390043-01</t>
+  </si>
+  <si>
+    <t>Shorting Bars</t>
+  </si>
+  <si>
+    <t>Jumpers</t>
+  </si>
+  <si>
+    <t>200-SNT100BKG</t>
+  </si>
+  <si>
+    <t>J100 J104 J151 J212 J213 J214 J351 J352 J500 J501 J502 J850 J852</t>
+  </si>
+  <si>
+    <t>Sockets (optional)</t>
   </si>
   <si>
     <t>390719-01</t>
@@ -1648,61 +1705,25 @@
     <t>U150 U211 U450 U700 U890</t>
   </si>
   <si>
-    <t>Various</t>
-  </si>
-  <si>
-    <t>391138-05</t>
-  </si>
-  <si>
-    <t>Inductor, 47µH</t>
-  </si>
-  <si>
-    <t>L500 can be left out on Acill boards</t>
-  </si>
-  <si>
-    <t>963-CBC3225T470MRV</t>
-  </si>
-  <si>
-    <t>L500</t>
-  </si>
-  <si>
-    <t>390924-01</t>
-  </si>
-  <si>
-    <t>Varistor Switch, Self Resetting 1.85A</t>
-  </si>
-  <si>
-    <t>652-MFR185</t>
-  </si>
-  <si>
-    <t>F175</t>
-  </si>
-  <si>
-    <t>380393-02</t>
-  </si>
-  <si>
-    <t>Battery, NiCd 3.6V 680mAh 3/60DK</t>
-  </si>
-  <si>
-    <t>Not recommended</t>
-  </si>
-  <si>
-    <t>BT176</t>
-  </si>
-  <si>
-    <t>390043-01</t>
-  </si>
-  <si>
-    <t>Shorting Bars</t>
-  </si>
-  <si>
-    <t>Jumpers</t>
-  </si>
-  <si>
-    <t>200-SNT100BKG</t>
-  </si>
-  <si>
-    <t>J100 J104 J151 J212 J213 J214 J351 J352 J500 J501 J502 J850 J852</t>
+    <t>Power Plug (optional)</t>
+  </si>
+  <si>
+    <t>Mate-N-Lok 6P Plug Housing</t>
+  </si>
+  <si>
+    <t>Counterpart for CN160</t>
+  </si>
+  <si>
+    <t>571-14807049</t>
+  </si>
+  <si>
+    <t>Mate-N-Lok Pin 20-14 AWG</t>
+  </si>
+  <si>
+    <t>Matching pins, crimping tool required</t>
+  </si>
+  <si>
+    <t>571-3505471</t>
   </si>
   <si>
     <r>
@@ -1724,7 +1745,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Version: 0.13 (2021-05-12)
+      <t xml:space="preserve">Version: 0.14 (2021-05-28)
 </t>
     </r>
     <r>
@@ -2158,7 +2179,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G146"/>
+  <dimension ref="A1:G149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4625,261 +4646,258 @@
         <v>511</v>
       </c>
       <c r="B131">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C131" t="s">
         <v>512</v>
       </c>
       <c r="D131" t="s">
-        <v>426</v>
+        <v>513</v>
+      </c>
+      <c r="E131" t="s">
+        <v>266</v>
       </c>
       <c r="F131" s="4" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="132" spans="1:7">
+      <c r="A132" t="s">
+        <v>516</v>
+      </c>
       <c r="B132">
         <v>1</v>
       </c>
       <c r="C132" t="s">
-        <v>515</v>
-      </c>
-      <c r="D132" t="s">
-        <v>516</v>
-      </c>
-      <c r="E132" t="s">
-        <v>51</v>
+        <v>517</v>
       </c>
       <c r="F132" s="4" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>52</v>
+        <v>519</v>
       </c>
     </row>
     <row r="133" spans="1:7">
       <c r="A133" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="B133">
         <v>1</v>
       </c>
       <c r="C133" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="D133" t="s">
-        <v>520</v>
-      </c>
-      <c r="E133" t="s">
-        <v>167</v>
-      </c>
-      <c r="F133" s="4" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>169</v>
+        <v>523</v>
       </c>
     </row>
     <row r="134" spans="1:7">
       <c r="A134" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B134">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C134" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="D134" t="s">
-        <v>524</v>
-      </c>
-      <c r="E134" t="s">
-        <v>44</v>
+        <v>526</v>
       </c>
       <c r="F134" s="4" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="135" spans="1:7">
-      <c r="B135">
-        <v>5</v>
-      </c>
-      <c r="C135" t="s">
-        <v>527</v>
-      </c>
-      <c r="D135" t="s">
-        <v>528</v>
-      </c>
-      <c r="E135" t="s">
-        <v>69</v>
-      </c>
-      <c r="F135" s="4" t="s">
+      <c r="A135" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G135" s="3" t="s">
+      <c r="B135" s="2"/>
+      <c r="C135" s="2"/>
+      <c r="D135" s="2"/>
+      <c r="E135" s="2"/>
+      <c r="F135" s="2"/>
+      <c r="G135" s="2"/>
+    </row>
+    <row r="136" spans="1:7">
+      <c r="A136" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="136" spans="1:7">
       <c r="B136">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C136" t="s">
         <v>531</v>
       </c>
       <c r="D136" t="s">
-        <v>528</v>
-      </c>
-      <c r="E136" t="s">
-        <v>63</v>
+        <v>426</v>
       </c>
       <c r="F136" s="4" t="s">
         <v>532</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>65</v>
+        <v>533</v>
       </c>
     </row>
     <row r="137" spans="1:7">
       <c r="B137">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C137" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="D137" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="E137" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="F137" s="4" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>536</v>
+        <v>52</v>
       </c>
     </row>
     <row r="138" spans="1:7">
+      <c r="A138" t="s">
+        <v>537</v>
+      </c>
       <c r="B138">
         <v>1</v>
       </c>
       <c r="C138" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="D138" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E138" t="s">
-        <v>21</v>
+        <v>167</v>
       </c>
       <c r="F138" s="4" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>22</v>
+        <v>169</v>
       </c>
     </row>
     <row r="139" spans="1:7">
+      <c r="A139" t="s">
+        <v>541</v>
+      </c>
       <c r="B139">
+        <v>2</v>
+      </c>
+      <c r="C139" t="s">
+        <v>542</v>
+      </c>
+      <c r="D139" t="s">
+        <v>543</v>
+      </c>
+      <c r="E139" t="s">
+        <v>44</v>
+      </c>
+      <c r="F139" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="G139" s="3" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
+      <c r="B140">
         <v>5</v>
       </c>
-      <c r="C139" t="s">
-        <v>540</v>
-      </c>
-      <c r="D139" t="s">
-        <v>541</v>
-      </c>
-      <c r="E139" t="s">
-        <v>14</v>
-      </c>
-      <c r="F139" s="4" t="s">
-        <v>542</v>
-      </c>
-      <c r="G139" s="3" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7">
-      <c r="A140" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="B140" s="2"/>
-      <c r="C140" s="2"/>
-      <c r="D140" s="2"/>
-      <c r="E140" s="2"/>
-      <c r="F140" s="2"/>
-      <c r="G140" s="2"/>
+      <c r="C140" t="s">
+        <v>546</v>
+      </c>
+      <c r="D140" t="s">
+        <v>547</v>
+      </c>
+      <c r="E140" t="s">
+        <v>69</v>
+      </c>
+      <c r="F140" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="141" spans="1:7">
-      <c r="A141" t="s">
-        <v>545</v>
-      </c>
       <c r="B141">
         <v>1</v>
       </c>
       <c r="C141" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="D141" t="s">
         <v>547</v>
       </c>
       <c r="E141" t="s">
-        <v>266</v>
+        <v>63</v>
       </c>
       <c r="F141" s="4" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>549</v>
+        <v>65</v>
       </c>
     </row>
     <row r="142" spans="1:7">
-      <c r="A142" t="s">
-        <v>550</v>
-      </c>
       <c r="B142">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C142" t="s">
-        <v>551</v>
+        <v>552</v>
+      </c>
+      <c r="D142" t="s">
+        <v>553</v>
+      </c>
+      <c r="E142" t="s">
+        <v>25</v>
       </c>
       <c r="F142" s="4" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="143" spans="1:7">
-      <c r="A143" t="s">
-        <v>554</v>
-      </c>
       <c r="B143">
         <v>1</v>
       </c>
       <c r="C143" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D143" t="s">
-        <v>556</v>
+        <v>557</v>
+      </c>
+      <c r="E143" t="s">
+        <v>21</v>
+      </c>
+      <c r="F143" s="4" t="s">
+        <v>558</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>557</v>
+        <v>22</v>
       </c>
     </row>
     <row r="144" spans="1:7">
-      <c r="A144" t="s">
-        <v>558</v>
-      </c>
       <c r="B144">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C144" t="s">
         <v>559</v>
@@ -4887,6 +4905,9 @@
       <c r="D144" t="s">
         <v>560</v>
       </c>
+      <c r="E144" t="s">
+        <v>14</v>
+      </c>
       <c r="F144" s="4" t="s">
         <v>561</v>
       </c>
@@ -4894,13 +4915,52 @@
         <v>562</v>
       </c>
     </row>
-    <row r="146" spans="1:1" ht="60" customHeight="1">
-      <c r="A146" s="5" t="s">
+    <row r="145" spans="1:7">
+      <c r="A145" s="2" t="s">
         <v>563</v>
       </c>
+      <c r="B145" s="2"/>
+      <c r="C145" s="2"/>
+      <c r="D145" s="2"/>
+      <c r="E145" s="2"/>
+      <c r="F145" s="2"/>
+      <c r="G145" s="2"/>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="B146">
+        <v>1</v>
+      </c>
+      <c r="C146" t="s">
+        <v>564</v>
+      </c>
+      <c r="D146" t="s">
+        <v>565</v>
+      </c>
+      <c r="F146" s="4" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="B147">
+        <v>6</v>
+      </c>
+      <c r="C147" t="s">
+        <v>567</v>
+      </c>
+      <c r="D147" t="s">
+        <v>568</v>
+      </c>
+      <c r="F147" s="4" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" ht="60" customHeight="1">
+      <c r="A149" s="5" t="s">
+        <v>570</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A13:G13"/>
@@ -4912,8 +4972,9 @@
     <mergeCell ref="A108:G108"/>
     <mergeCell ref="A113:G113"/>
     <mergeCell ref="A130:G130"/>
-    <mergeCell ref="A140:G140"/>
-    <mergeCell ref="A146:G146"/>
+    <mergeCell ref="A135:G135"/>
+    <mergeCell ref="A145:G145"/>
+    <mergeCell ref="A149:G149"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F19" r:id="rId1"/>
@@ -5016,16 +5077,18 @@
     <hyperlink ref="F128" r:id="rId98"/>
     <hyperlink ref="F131" r:id="rId99"/>
     <hyperlink ref="F132" r:id="rId100"/>
-    <hyperlink ref="F133" r:id="rId101"/>
-    <hyperlink ref="F134" r:id="rId102"/>
-    <hyperlink ref="F135" r:id="rId103"/>
-    <hyperlink ref="F136" r:id="rId104"/>
-    <hyperlink ref="F137" r:id="rId105"/>
-    <hyperlink ref="F138" r:id="rId106"/>
-    <hyperlink ref="F139" r:id="rId107"/>
-    <hyperlink ref="F141" r:id="rId108"/>
-    <hyperlink ref="F142" r:id="rId109"/>
+    <hyperlink ref="F134" r:id="rId101"/>
+    <hyperlink ref="F136" r:id="rId102"/>
+    <hyperlink ref="F137" r:id="rId103"/>
+    <hyperlink ref="F138" r:id="rId104"/>
+    <hyperlink ref="F139" r:id="rId105"/>
+    <hyperlink ref="F140" r:id="rId106"/>
+    <hyperlink ref="F141" r:id="rId107"/>
+    <hyperlink ref="F142" r:id="rId108"/>
+    <hyperlink ref="F143" r:id="rId109"/>
     <hyperlink ref="F144" r:id="rId110"/>
+    <hyperlink ref="F146" r:id="rId111"/>
+    <hyperlink ref="F147" r:id="rId112"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Remark replacement for HN62402
</commit_message>
<xml_diff>
--- a/docs/a4000-bom.xlsx
+++ b/docs/a4000-bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="572">
   <si>
     <t>Part Id</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>HN62402, 150ns, Kickstart ROM "Low"</t>
+  </si>
+  <si>
+    <t>Replace with AM27C400, MX27C4100 or similar</t>
   </si>
   <si>
     <t>DIP40</t>
@@ -2416,742 +2419,748 @@
       <c r="C14" t="s">
         <v>43</v>
       </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
         <v>25</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E25" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E26" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E27" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E28" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E30" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E31" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E32" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E33" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E34" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E35" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E36" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E37" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E38" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B39">
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E39" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E40" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B41">
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E41" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E42" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E43" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B44">
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E44" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B45">
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E45" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E46" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E47" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E48" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B49">
         <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E49" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B50">
         <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E50" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -3162,67 +3171,67 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B52">
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E52" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B53">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E53" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B54">
         <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E54" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -3233,47 +3242,47 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B56">
         <v>15</v>
       </c>
       <c r="C56" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E56" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B57">
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E57" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -3284,367 +3293,367 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B59">
         <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E59" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B60">
         <v>29</v>
       </c>
       <c r="C60" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E60" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B61">
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E61" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B62">
         <v>44</v>
       </c>
       <c r="C62" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E62" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B63">
         <v>2</v>
       </c>
       <c r="C63" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E63" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B64">
         <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E64" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B65">
         <v>2</v>
       </c>
       <c r="C65" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E65" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B66">
         <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E66" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B67">
         <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E67" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B68">
         <v>64</v>
       </c>
       <c r="C68" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E68" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B69">
         <v>19</v>
       </c>
       <c r="C69" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E69" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B70">
         <v>2</v>
       </c>
       <c r="C70" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E70" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B71">
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E71" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B72">
         <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E72" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B73">
         <v>10</v>
       </c>
       <c r="C73" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E73" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B74">
         <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E74" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B75">
         <v>2</v>
       </c>
       <c r="C75" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E75" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B76">
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E76" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -3655,550 +3664,550 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B78">
         <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E78" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B79">
         <v>2</v>
       </c>
       <c r="C79" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E79" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B80">
         <v>1</v>
       </c>
       <c r="C80" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E80" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B81">
         <v>3</v>
       </c>
       <c r="C81" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D81" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E81" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B82">
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E82" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B83">
         <v>37</v>
       </c>
       <c r="C83" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E83" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B84">
         <v>117</v>
       </c>
       <c r="C84" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E84" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B85">
         <v>24</v>
       </c>
       <c r="C85" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E85" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B86">
         <v>3</v>
       </c>
       <c r="C86" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E86" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B87">
         <v>2</v>
       </c>
       <c r="C87" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E87" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B88">
         <v>6</v>
       </c>
       <c r="C88" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E88" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B89">
         <v>2</v>
       </c>
       <c r="C89" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E89" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B90">
         <v>2</v>
       </c>
       <c r="C90" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E90" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B91">
         <v>66</v>
       </c>
       <c r="C91" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E91" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B92">
         <v>12</v>
       </c>
       <c r="C92" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E92" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B93">
         <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E93" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B94">
         <v>76</v>
       </c>
       <c r="C94" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E94" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B95">
         <v>3</v>
       </c>
       <c r="C95" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E95" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B96">
         <v>17</v>
       </c>
       <c r="C96" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="E96" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B97">
         <v>21</v>
       </c>
       <c r="C97" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E97" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B98">
         <v>2</v>
       </c>
       <c r="C98" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E98" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B99">
         <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E99" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B100">
         <v>2</v>
       </c>
       <c r="C100" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E100" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B101">
         <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="E101" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B102">
         <v>3</v>
       </c>
       <c r="C102" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="E102" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B103">
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E103" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B104">
         <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E104" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -4209,47 +4218,47 @@
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B106">
         <v>12</v>
       </c>
       <c r="C106" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E106" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B107">
         <v>17</v>
       </c>
       <c r="C107" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E107" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -4260,87 +4269,87 @@
     </row>
     <row r="109" spans="1:7">
       <c r="A109" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B109">
         <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E109" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B110">
         <v>1</v>
       </c>
       <c r="C110" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D110" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="E110" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" t="s">
+        <v>436</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="C111" t="s">
+        <v>437</v>
+      </c>
+      <c r="D111" t="s">
+        <v>438</v>
+      </c>
+      <c r="E111" t="s">
+        <v>59</v>
+      </c>
+      <c r="G111" s="3" t="s">
         <v>435</v>
-      </c>
-      <c r="B111">
-        <v>1</v>
-      </c>
-      <c r="C111" t="s">
-        <v>436</v>
-      </c>
-      <c r="D111" t="s">
-        <v>437</v>
-      </c>
-      <c r="E111" t="s">
-        <v>58</v>
-      </c>
-      <c r="G111" s="3" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B112">
         <v>1</v>
       </c>
       <c r="C112" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E112" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -4351,288 +4360,288 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B114">
         <v>5</v>
       </c>
       <c r="C114" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="115" spans="1:7">
       <c r="A115" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B115">
         <v>1</v>
       </c>
       <c r="C115" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="116" spans="1:7">
       <c r="A116" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B116">
         <v>1</v>
       </c>
       <c r="C116" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="117" spans="1:7">
       <c r="A117" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B117">
         <v>1</v>
       </c>
       <c r="C117" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="118" spans="1:7">
       <c r="A118" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B118">
         <v>2</v>
       </c>
       <c r="C118" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B119">
         <v>15</v>
       </c>
       <c r="C119" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="120" spans="1:7">
       <c r="A120" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B120">
         <v>2</v>
       </c>
       <c r="C120" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D120" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="121" spans="1:7">
       <c r="A121" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B121">
         <v>1</v>
       </c>
       <c r="C121" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D121" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="122" spans="1:7">
       <c r="A122" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B122">
         <v>1</v>
       </c>
       <c r="C122" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D122" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="123" spans="1:7">
       <c r="A123" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B123">
         <v>1</v>
       </c>
       <c r="C123" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D123" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="124" spans="1:7">
       <c r="A124" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B124">
         <v>1</v>
       </c>
       <c r="C124" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="125" spans="1:7">
       <c r="A125" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B125">
         <v>1</v>
       </c>
       <c r="C125" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="D125" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="126" spans="1:7">
       <c r="A126" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B126">
         <v>1</v>
       </c>
       <c r="C126" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="D126" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="127" spans="1:7">
       <c r="A127" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B127">
         <v>1</v>
       </c>
       <c r="C127" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="D127" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F127" s="4" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="128" spans="1:7">
       <c r="A128" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B128">
         <v>2</v>
       </c>
       <c r="C128" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="129" spans="1:7">
       <c r="A129" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B129">
         <v>1</v>
       </c>
       <c r="C129" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="130" spans="1:7">
       <c r="A130" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -4643,84 +4652,84 @@
     </row>
     <row r="131" spans="1:7">
       <c r="A131" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B131">
         <v>1</v>
       </c>
       <c r="C131" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D131" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="E131" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F131" s="4" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="132" spans="1:7">
       <c r="A132" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B132">
         <v>1</v>
       </c>
       <c r="C132" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="F132" s="4" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="133" spans="1:7">
       <c r="A133" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B133">
         <v>1</v>
       </c>
       <c r="C133" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D133" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="134" spans="1:7">
       <c r="A134" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B134">
         <v>13</v>
       </c>
       <c r="C134" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="D134" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="F134" s="4" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="135" spans="1:7">
       <c r="A135" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -4731,22 +4740,22 @@
     </row>
     <row r="136" spans="1:7">
       <c r="A136" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B136">
         <v>8</v>
       </c>
       <c r="C136" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D136" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="F136" s="4" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -4754,65 +4763,65 @@
         <v>1</v>
       </c>
       <c r="C137" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D137" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E137" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F137" s="4" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="138" spans="1:7">
       <c r="A138" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B138">
         <v>1</v>
       </c>
       <c r="C138" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D138" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E138" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F138" s="4" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="139" spans="1:7">
       <c r="A139" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B139">
         <v>2</v>
       </c>
       <c r="C139" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D139" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E139" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F139" s="4" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -4820,19 +4829,19 @@
         <v>5</v>
       </c>
       <c r="C140" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="D140" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E140" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F140" s="4" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -4840,19 +4849,19 @@
         <v>1</v>
       </c>
       <c r="C141" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D141" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E141" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F141" s="4" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -4860,19 +4869,19 @@
         <v>3</v>
       </c>
       <c r="C142" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="D142" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="E142" t="s">
         <v>25</v>
       </c>
       <c r="F142" s="4" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -4880,16 +4889,16 @@
         <v>1</v>
       </c>
       <c r="C143" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="D143" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E143" t="s">
         <v>21</v>
       </c>
       <c r="F143" s="4" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="G143" s="3" t="s">
         <v>22</v>
@@ -4900,24 +4909,24 @@
         <v>5</v>
       </c>
       <c r="C144" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D144" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E144" t="s">
         <v>14</v>
       </c>
       <c r="F144" s="4" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="145" spans="1:7">
       <c r="A145" s="2" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -4931,13 +4940,13 @@
         <v>1</v>
       </c>
       <c r="C146" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="D146" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="F146" s="4" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -4945,18 +4954,18 @@
         <v>6</v>
       </c>
       <c r="C147" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D147" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="F147" s="4" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="60" customHeight="1">
       <c r="A149" s="5" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>